<commit_message>
add dependencies for windows
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewpaulikas/repos/excel-spliter/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\repos\excel-spliter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A58ED204-19BB-AE47-AA1B-27D398FD825E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C47719A-CE94-4121-A9D2-B2A565108800}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{058A3C0E-B94E-AD44-A9BF-792392B6A6D9}"/>
+    <workbookView xWindow="28680" yWindow="285" windowWidth="29040" windowHeight="15465" xr2:uid="{058A3C0E-B94E-AD44-A9BF-792392B6A6D9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -443,21 +443,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76EA2242-DEA5-BC4C-B4BA-493DF6107967}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -474,7 +474,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -491,7 +491,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -508,7 +508,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -523,11 +523,6 @@
       </c>
       <c r="E4" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -543,15 +538,15 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -568,7 +563,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -585,7 +580,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -602,7 +597,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -632,15 +627,15 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -657,7 +652,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -674,7 +669,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -691,7 +686,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>

</xml_diff>